<commit_message>
allow the model to set initial market asset value to a percentage of AL.
</commit_message>
<xml_diff>
--- a/RunControl_test.xlsx
+++ b/RunControl_test.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="173">
   <si>
     <t>Sheet #</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Method 1 (PSERS): The difference between expected and actual investment return will be realized over s.year years. (realize 1/s.year each year)</t>
   </si>
   <si>
-    <t>Method 2 (TPAF):  "MA" for preset value; "AL" for being equal to initial liability</t>
-  </si>
-  <si>
     <t>Method 2 (TPAF): expected market value at 0. Set to the same value as MA_0 by default. expected market value at 0. Set to the same value as MA_0 by default</t>
   </si>
   <si>
@@ -536,6 +533,21 @@
   </si>
   <si>
     <t>Non-Negative ADC and ERC</t>
+  </si>
+  <si>
+    <t>How initial MA is determined</t>
+  </si>
+  <si>
+    <t>"MA" for preset value; "AL" for being equal to initial liability;""AL_pct being % of AL</t>
+  </si>
+  <si>
+    <t>MA_0_pct</t>
+  </si>
+  <si>
+    <t>MV assets at time 0 as a % of AL</t>
+  </si>
+  <si>
+    <t>AL_pct</t>
   </si>
 </sst>
 </file>
@@ -731,11 +743,11 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1238,13 +1250,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO8"/>
+  <dimension ref="A1:AP15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="X6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AH6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AH3" sqref="AH3"/>
+      <selection pane="bottomRight" activeCell="AU4" sqref="AU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,15 +1272,14 @@
     <col min="17" max="21" width="12.7109375"/>
     <col min="22" max="22" width="11.140625" customWidth="1"/>
     <col min="23" max="32" width="12.7109375"/>
-    <col min="35" max="35" width="12.7109375"/>
-    <col min="36" max="38" width="27.140625"/>
-    <col min="39" max="39" width="20.7109375"/>
-    <col min="40" max="40" width="26.85546875"/>
-    <col min="41" max="41" width="16"/>
-    <col min="42" max="1028" width="8.5703125"/>
+    <col min="36" max="36" width="11.28515625" customWidth="1"/>
+    <col min="38" max="38" width="16.7109375" customWidth="1"/>
+    <col min="39" max="39" width="15.7109375" customWidth="1"/>
+    <col min="40" max="40" width="10.140625" customWidth="1"/>
+    <col min="43" max="1007" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1278,7 +1289,7 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
     </row>
-    <row r="2" spans="1:41" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1340,20 +1351,25 @@
         <v>40</v>
       </c>
       <c r="AH2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AI2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
       <c r="AL2" s="6"/>
       <c r="AM2" s="6"/>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1387,46 +1403,47 @@
       <c r="AE3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ3" s="4"/>
+      <c r="AM3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AO3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="29"/>
       <c r="L4" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
@@ -1435,196 +1452,200 @@
       <c r="Q4" s="28"/>
       <c r="R4" s="28"/>
       <c r="S4" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T4" s="29"/>
       <c r="U4" s="29"/>
       <c r="V4" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W4" s="30"/>
       <c r="X4" s="30"/>
       <c r="Y4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="Z4" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="AA4" s="25"/>
       <c r="AB4" s="25"/>
-      <c r="AC4" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
+      <c r="AC4" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
       <c r="AG4" s="17"/>
       <c r="AH4" s="18"/>
       <c r="AI4" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="AJ4" s="30"/>
-      <c r="AK4" s="31" t="s">
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
+      <c r="AO4" s="32"/>
+      <c r="AP4" s="32"/>
+    </row>
+    <row r="5" spans="1:42" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="AL4" s="31"/>
-      <c r="AM4" s="31"/>
-      <c r="AN4" s="31"/>
-      <c r="AO4" s="31"/>
-    </row>
-    <row r="5" spans="1:41" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="V5" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="V5" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG5" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="AH5" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AJ5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AM5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN5" s="9" t="s">
+      <c r="AP5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AO5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
       </c>
       <c r="C6" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
         <v>112</v>
       </c>
-      <c r="E6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>113</v>
-      </c>
-      <c r="I6" t="s">
-        <v>114</v>
       </c>
       <c r="J6" s="12">
         <v>0</v>
@@ -1663,7 +1684,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -1672,19 +1693,19 @@
         <v>0.12</v>
       </c>
       <c r="Y6" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="AB6">
         <v>3</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD6" s="14">
         <v>0.25</v>
@@ -1701,56 +1722,59 @@
       <c r="AH6" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ6" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="AK6">
         <v>200</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AL6" t="s">
         <v>119</v>
       </c>
-      <c r="AK6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>10</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="AN6">
         <v>200</v>
       </c>
-      <c r="AO6">
+      <c r="AO6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
         <v>112</v>
       </c>
-      <c r="E7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>113</v>
-      </c>
-      <c r="I7" t="s">
-        <v>114</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
@@ -1789,7 +1813,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V7" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W7" s="12">
         <v>7.4999999999999997E-2</v>
@@ -1798,19 +1822,19 @@
         <v>0.12</v>
       </c>
       <c r="Y7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="AB7">
         <v>3</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD7" s="14">
         <v>0.25</v>
@@ -1827,56 +1851,59 @@
       <c r="AH7" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ7" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="AK7">
         <v>200</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AL7" t="s">
         <v>119</v>
       </c>
-      <c r="AK7" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>10</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="AN7">
         <v>200</v>
       </c>
-      <c r="AO7">
+      <c r="AO7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
         <v>112</v>
       </c>
-      <c r="E8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>113</v>
-      </c>
-      <c r="I8" t="s">
-        <v>114</v>
       </c>
       <c r="J8" s="12">
         <v>0</v>
@@ -1915,7 +1942,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W8" s="12">
         <v>7.4999999999999997E-2</v>
@@ -1924,19 +1951,19 @@
         <v>0.12</v>
       </c>
       <c r="Y8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="AB8">
         <v>3</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD8" s="14">
         <v>0.25</v>
@@ -1953,50 +1980,79 @@
       <c r="AH8" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ8" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="AK8">
         <v>200</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AL8" t="s">
         <v>119</v>
       </c>
-      <c r="AK8" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>10</v>
-      </c>
-      <c r="AM8" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="AN8">
         <v>200</v>
       </c>
-      <c r="AO8">
+      <c r="AO8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP8">
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="21"/>
+      <c r="AO9" s="2"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="21"/>
+      <c r="AO10" s="2"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="21"/>
+      <c r="AO11" s="2"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="21"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="21"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="21"/>
+      <c r="AO14" s="2"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="21"/>
+      <c r="AO15" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AO4"/>
+  <mergeCells count="11">
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
   </mergeCells>
-  <dataValidations count="19">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ8">
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO14:AO15">
       <formula1>"MA,EAA"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM8">
-      <formula1>"MA,AL"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA8">
@@ -2047,21 +2103,28 @@
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AL6:AL8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AM6:AM11 AM14:AM15">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN14:AN15 AN6:AN11">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO8">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP14:AP15">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH8">
       <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ15">
+      <formula1>0</formula1>
+      <formula2>1.5</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI15">
+      <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -2084,21 +2147,21 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2112,7 +2175,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="12">
         <v>5.5E-2</v>
@@ -2126,7 +2189,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2165,21 +2228,21 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="20">
         <v>11</v>
@@ -2193,7 +2256,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="20">
         <v>20</v>
@@ -2225,30 +2288,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,7 +2361,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2308,228 +2371,228 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
         <v>138</v>
-      </c>
-      <c r="C9" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" t="s">
         <v>141</v>
-      </c>
-      <c r="C13" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
         <v>143</v>
-      </c>
-      <c r="C14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" t="s">
         <v>146</v>
-      </c>
-      <c r="C18" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" t="s">
         <v>146</v>
-      </c>
-      <c r="C22" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" t="s">
         <v>146</v>
-      </c>
-      <c r="C26" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s">
         <v>146</v>
-      </c>
-      <c r="C30" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" t="s">
         <v>149</v>
-      </c>
-      <c r="C34" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" t="s">
         <v>152</v>
-      </c>
-      <c r="C38" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" t="s">
         <v>154</v>
-      </c>
-      <c r="C39" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" t="s">
         <v>156</v>
-      </c>
-      <c r="C40" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set nsim to 1 when using deterministic return
</commit_message>
<xml_diff>
--- a/RunControl_test.xlsx
+++ b/RunControl_test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -725,7 +725,22 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -733,21 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1109,14 +1109,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125"/>
-    <col min="2" max="2" width="16.7109375"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="7.5546875"/>
+    <col min="2" max="2" width="16.6640625"/>
+    <col min="3" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1167,77 +1167,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1253,33 +1253,33 @@
   <dimension ref="A1:AP15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AH6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AU4" sqref="AU4"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.42578125"/>
-    <col min="2" max="2" width="19.7109375"/>
-    <col min="3" max="9" width="24.42578125"/>
-    <col min="10" max="11" width="17.42578125"/>
-    <col min="12" max="12" width="16.140625"/>
-    <col min="13" max="14" width="21.42578125"/>
-    <col min="15" max="15" width="24.5703125"/>
+    <col min="1" max="1" width="54.44140625"/>
+    <col min="2" max="2" width="19.6640625"/>
+    <col min="3" max="9" width="24.44140625"/>
+    <col min="10" max="11" width="17.44140625"/>
+    <col min="12" max="12" width="16.109375"/>
+    <col min="13" max="14" width="21.44140625"/>
+    <col min="15" max="15" width="24.5546875"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.7109375"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
-    <col min="23" max="32" width="12.7109375"/>
-    <col min="36" max="36" width="11.28515625" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" customWidth="1"/>
-    <col min="39" max="39" width="15.7109375" customWidth="1"/>
-    <col min="40" max="40" width="10.140625" customWidth="1"/>
-    <col min="43" max="1007" width="8.5703125"/>
+    <col min="17" max="21" width="12.6640625"/>
+    <col min="22" max="22" width="11.109375" customWidth="1"/>
+    <col min="23" max="32" width="12.6640625"/>
+    <col min="36" max="36" width="11.33203125" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" customWidth="1"/>
+    <col min="40" max="40" width="10.109375" customWidth="1"/>
+    <col min="43" max="1007" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
     </row>
-    <row r="2" spans="1:42" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1420,42 +1420,42 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:42" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="28" t="s">
+      <c r="K4" s="27"/>
+      <c r="L4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="29" t="s">
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
       <c r="V4" s="30" t="s">
         <v>65</v>
       </c>
@@ -1464,17 +1464,17 @@
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="31" t="s">
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
       <c r="AG4" s="17"/>
       <c r="AH4" s="18"/>
       <c r="AI4" s="30" t="s">
@@ -1482,15 +1482,15 @@
       </c>
       <c r="AJ4" s="30"/>
       <c r="AK4" s="30"/>
-      <c r="AL4" s="32" t="s">
+      <c r="AL4" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AM4" s="32"/>
-      <c r="AN4" s="32"/>
-      <c r="AO4" s="32"/>
-      <c r="AP4" s="32"/>
-    </row>
-    <row r="5" spans="1:42" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+    </row>
+    <row r="5" spans="1:42" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="X6" s="12">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
         <v>114</v>
@@ -1747,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -2005,50 +2005,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AI9" s="2"/>
       <c r="AJ9" s="21"/>
       <c r="AO9" s="2"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AI10" s="2"/>
       <c r="AJ10" s="21"/>
       <c r="AO10" s="2"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AI11" s="2"/>
       <c r="AJ11" s="21"/>
       <c r="AO11" s="2"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AJ12" s="21"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AJ13" s="21"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AI14" s="2"/>
       <c r="AJ14" s="21"/>
       <c r="AO14" s="2"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AI15" s="2"/>
       <c r="AJ15" s="21"/>
       <c r="AO15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="V4:X4"/>
     <mergeCell ref="AI4:AK4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO14:AO15">
@@ -2143,9 +2143,9 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -2224,9 +2224,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -2281,17 +2281,17 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>105</v>
       </c>
@@ -2351,30 +2351,30 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125"/>
+    <col min="1" max="1" width="23.44140625"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.42578125"/>
-    <col min="4" max="1025" width="8.5703125"/>
+    <col min="3" max="3" width="85.44140625"/>
+    <col min="4" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>133</v>
       </c>
@@ -2382,12 +2382,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -2411,12 +2411,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -2440,12 +2440,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>111</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -2461,12 +2461,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2482,12 +2482,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -2503,12 +2503,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -2524,12 +2524,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>148</v>
       </c>
@@ -2545,12 +2545,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -2582,12 +2582,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>113</v>
       </c>

</xml_diff>